<commit_message>
Updated Venn diagram and shared OTUs to 0.01% abundance threshold.
</commit_message>
<xml_diff>
--- a/Tables/Shared_otus.xlsx
+++ b/Tables/Shared_otus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/liberjul_msu_edu/Documents/Documents/MSU/Undergrad/Fall 2018/PLP 847/miseq_dat/Leaf_litter_communities/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3694B93F-4459-423B-9FE1-3621A74D93CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ABC563F-7DF9-4C29-A228-2CA384894756}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33540" yWindow="6795" windowWidth="6405" windowHeight="3345"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Shared_otus" sheetId="1" r:id="rId1"/>
@@ -55,16 +55,16 @@
     <t>Total Shared</t>
   </si>
   <si>
-    <t>452 (79%)</t>
-  </si>
-  <si>
-    <t>256 (97%)</t>
-  </si>
-  <si>
-    <t>572 (80%)</t>
-  </si>
-  <si>
-    <t>226 (30%)</t>
+    <t>263 (98%)</t>
+  </si>
+  <si>
+    <t>200 (99%)</t>
+  </si>
+  <si>
+    <t>357 (85%)</t>
+  </si>
+  <si>
+    <t>152 (42%)</t>
   </si>
 </sst>
 </file>
@@ -907,12 +907,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
@@ -933,16 +932,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>570</v>
+        <v>268</v>
       </c>
       <c r="C2">
-        <v>264</v>
+        <v>202</v>
       </c>
       <c r="D2">
-        <v>719</v>
+        <v>421</v>
       </c>
       <c r="E2">
-        <v>759</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -950,16 +949,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>147</v>
+        <v>64</v>
       </c>
       <c r="E3">
-        <v>533</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -970,13 +969,13 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>227</v>
+        <v>180</v>
       </c>
       <c r="D4">
-        <v>352</v>
+        <v>247</v>
       </c>
       <c r="E4">
-        <v>88</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -984,16 +983,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>227</v>
+        <v>180</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5">
-        <v>223</v>
+        <v>187</v>
       </c>
       <c r="E5">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1001,16 +1000,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>352</v>
+        <v>247</v>
       </c>
       <c r="C6">
-        <v>223</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6">
-        <v>195</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1033,245 +1032,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AFDA51084187F242B05EFA296C5963FF" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3643f2840fd34a552c287b84deed346">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3ea71f81-dc8a-4f4b-b0dd-c828e930e924" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bc954b55e77a02dd874654cc5b225bc" ns3:_="">
-    <xsd:import namespace="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3ea71f81-dc8a-4f4b-b0dd-c828e930e924" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="12" nillable="true" ma:displayName="MediaServiceLocation" ma:description="" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53B1403D-755C-4635-8572-B92E570C749F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{953813DB-C838-41B8-9016-037B1B601C91}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1B2F934-AA6E-4A69-BB89-E9C6756A7692}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added percentages to shared otu table.
</commit_message>
<xml_diff>
--- a/Tables/Shared_otus.xlsx
+++ b/Tables/Shared_otus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/liberjul_msu_edu/Documents/Documents/MSU/Undergrad/Fall 2018/PLP 847/miseq_dat/Leaf_litter_communities/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ABC563F-7DF9-4C29-A228-2CA384894756}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{86C40C51-51E0-4F4C-AB56-810E45F52586}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Epiphyte</t>
   </si>
@@ -40,16 +40,55 @@
     <t>Unique OTUs</t>
   </si>
   <si>
+    <t>5 (2%)</t>
+  </si>
+  <si>
+    <t>2 (1%)</t>
+  </si>
+  <si>
+    <t>64 (15%)</t>
+  </si>
+  <si>
+    <t>212 (58%)</t>
+  </si>
+  <si>
     <t>Shared with Epiphytes</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
+    <t>180 (89%)</t>
+  </si>
+  <si>
+    <t>247 (59%)</t>
+  </si>
+  <si>
+    <t>57 (16%)</t>
+  </si>
+  <si>
     <t>Shared with Endophytes</t>
   </si>
   <si>
+    <t>180 (67%)</t>
+  </si>
+  <si>
+    <t>187 (44%)</t>
+  </si>
+  <si>
+    <t>43 (12%)</t>
+  </si>
+  <si>
     <t>Shared with Litter</t>
+  </si>
+  <si>
+    <t>247 (92%)</t>
+  </si>
+  <si>
+    <t>187 (93%)</t>
+  </si>
+  <si>
+    <t>145 (40%)</t>
   </si>
   <si>
     <t>Total Shared</t>
@@ -907,9 +946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -948,88 +985,329 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>64</v>
-      </c>
-      <c r="E3">
-        <v>212</v>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>180</v>
-      </c>
-      <c r="D4">
-        <v>247</v>
-      </c>
-      <c r="E4">
-        <v>57</v>
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>180</v>
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>187</v>
-      </c>
-      <c r="E5">
-        <v>43</v>
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>247</v>
-      </c>
-      <c r="C6">
-        <v>187</v>
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>145</v>
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AFDA51084187F242B05EFA296C5963FF" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3643f2840fd34a552c287b84deed346">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3ea71f81-dc8a-4f4b-b0dd-c828e930e924" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bc954b55e77a02dd874654cc5b225bc" ns3:_="">
+    <xsd:import namespace="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3ea71f81-dc8a-4f4b-b0dd-c828e930e924" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="12" nillable="true" ma:displayName="MediaServiceLocation" ma:description="" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6557F3DE-5795-4223-92E0-7DC9EE262879}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76A5600-742A-4E09-B2E8-CEAA35429EC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A19CA3CA-2529-4A4D-A396-2E32DE0E3F53}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added linear models instead of aov for model comprison, AICc comparison, and removed eigenvalue plotting. Increased Shared_otu.xlsx column width.
</commit_message>
<xml_diff>
--- a/Tables/Shared_otus.xlsx
+++ b/Tables/Shared_otus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/liberjul_msu_edu/Documents/Documents/MSU/Undergrad/Fall 2018/PLP 847/miseq_dat/Leaf_litter_communities/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\OneDrive - Michigan State University\Documents\MSU\Undergrad\Fall 2018\PLP 847\miseq_dat\Leaf_litter_communities\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86C40C51-51E0-4F4C-AB56-810E45F52586}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{86C40C51-51E0-4F4C-AB56-810E45F52586}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{6399C0B0-55FF-4536-9C80-F852EC05EFB5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shared_otus" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -943,12 +943,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
@@ -1072,6 +1075,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AFDA51084187F242B05EFA296C5963FF" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3643f2840fd34a552c287b84deed346">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3ea71f81-dc8a-4f4b-b0dd-c828e930e924" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bc954b55e77a02dd874654cc5b225bc" ns3:_="">
     <xsd:import namespace="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
@@ -1255,22 +1273,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A19CA3CA-2529-4A4D-A396-2E32DE0E3F53}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76A5600-742A-4E09-B2E8-CEAA35429EC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6557F3DE-5795-4223-92E0-7DC9EE262879}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1286,28 +1313,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76A5600-742A-4E09-B2E8-CEAA35429EC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A19CA3CA-2529-4A4D-A396-2E32DE0E3F53}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>